<commit_message>
changed bat files so that they used javac in jre directory tidied up nmrproblem.py updated todo list
</commit_message>
<xml_diff>
--- a/exampleProblems/ch9_016/ch9_016.xlsx
+++ b/exampleProblems/ch9_016/ch9_016.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/ch9_016/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="11_5573853B0C84BB957DF9412134EB6A4605B0F9D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C8B0118-764C-456D-BEFF-56C6EF01EB08}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_5573853B0C84BB957DF9412134EB6A4605B0F9D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA167CDF-6601-4377-9719-43B21577D9CC}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="1980" windowWidth="23880" windowHeight="13620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="1650" windowWidth="23880" windowHeight="13620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
     <sheet name="H1_1D" sheetId="1" r:id="rId2"/>
-    <sheet name="HSQC" sheetId="4" r:id="rId3"/>
-    <sheet name="NOESY" sheetId="11" r:id="rId4"/>
+    <sheet name="H1_pureshift" sheetId="3" r:id="rId3"/>
+    <sheet name="C13_1D" sheetId="2" r:id="rId4"/>
     <sheet name="COSY" sheetId="5" r:id="rId5"/>
-    <sheet name="HMBC" sheetId="8" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId7"/>
-    <sheet name="C13_1D" sheetId="2" r:id="rId8"/>
-    <sheet name="H1_pureshift" sheetId="3" r:id="rId9"/>
+    <sheet name="HSQC" sheetId="4" r:id="rId6"/>
+    <sheet name="HMBC" sheetId="8" r:id="rId7"/>
+    <sheet name="NOESY" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -587,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -624,13 +623,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -907,49 +906,43 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -957,31 +950,24 @@
         <v>3.75</v>
       </c>
       <c r="C2" s="1">
-        <v>57.4</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="1">
-        <v>0.2</v>
+        <v>1.76</v>
       </c>
       <c r="E2" s="1">
-        <v>10.63</v>
-      </c>
-      <c r="F2" s="1">
-        <v>35.96</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3.57</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="6"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>9.57</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -989,31 +975,24 @@
         <v>2.34</v>
       </c>
       <c r="C3" s="1">
-        <v>36.200000000000003</v>
+        <v>0.8</v>
       </c>
       <c r="D3" s="1">
-        <v>-0.2</v>
+        <v>1.61</v>
       </c>
       <c r="E3" s="1">
-        <v>18.68</v>
-      </c>
-      <c r="F3" s="1">
-        <v>38.54</v>
-      </c>
-      <c r="G3" s="1">
-        <v>6.34</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="6"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>14.49</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1021,31 +1000,24 @@
         <v>2.11</v>
       </c>
       <c r="C4" s="1">
-        <v>29.7</v>
+        <v>0.8</v>
       </c>
       <c r="D4" s="1">
-        <v>-0.2</v>
+        <v>1.61</v>
       </c>
       <c r="E4" s="1">
-        <v>8.69</v>
-      </c>
-      <c r="F4" s="1">
-        <v>35.15</v>
-      </c>
-      <c r="G4" s="1">
-        <v>3.16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="6"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>13.64</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1053,31 +1025,24 @@
         <v>2.06</v>
       </c>
       <c r="C5" s="1">
-        <v>29.7</v>
+        <v>0.9</v>
       </c>
       <c r="D5" s="1">
-        <v>-0.3</v>
+        <v>1.65</v>
       </c>
       <c r="E5" s="1">
-        <v>17.059999999999999</v>
-      </c>
-      <c r="F5" s="1">
-        <v>36.61</v>
-      </c>
-      <c r="G5" s="1">
-        <v>7.62</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="6"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>16.45</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1086,11 +1051,9 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1099,12 +1062,9 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="6"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1113,12 +1073,9 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="6"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1127,12 +1084,9 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="6"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1141,12 +1095,9 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="6"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1155,68 +1106,277 @@
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="9"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M15" s="8"/>
+      <c r="I11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0628732-26E0-6345-9202-8A755BCBA328}">
-  <dimension ref="A1:K1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>184.1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>381</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2520.89</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>177.4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>737.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2812.18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>57.4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>543.29999999999995</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2383.0100000000002</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2086.1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.01</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9387.2800000000007</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2093.5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="E6" s="1">
+        <v>8261.02</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1952,6 +2112,272 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="C2" s="1">
+        <v>57.4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10.63</v>
+      </c>
+      <c r="F2" s="1">
+        <v>35.96</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3.57</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="6"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="C3" s="1">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>18.68</v>
+      </c>
+      <c r="F3" s="1">
+        <v>38.54</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6.34</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8.69</v>
+      </c>
+      <c r="F4" s="1">
+        <v>35.15</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3.16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="6"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="C5" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-0.3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>17.059999999999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>36.61</v>
+      </c>
+      <c r="G5" s="1">
+        <v>7.62</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="6"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="6"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="6"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="6"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="6"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="9"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M15" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:V45"/>
   <sheetViews>
@@ -2835,487 +3261,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0628732-26E0-6345-9202-8A755BCBA328}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I15"/>
-  <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>184.1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>381</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.45</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2520.89</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>177.4</v>
-      </c>
-      <c r="C3" s="1">
-        <v>737.5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.89</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2812.18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>57.4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>543.29999999999995</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1.02</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2383.0100000000002</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2086.1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.01</v>
-      </c>
-      <c r="E5" s="1">
-        <v>9387.2800000000007</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>29.7</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2093.5</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.93</v>
-      </c>
-      <c r="E6" s="1">
-        <v>8261.02</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I11"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>3.75</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.76</v>
-      </c>
-      <c r="E2" s="1">
-        <v>9.57</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2.34</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1.61</v>
-      </c>
-      <c r="E3" s="1">
-        <v>14.49</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2.11</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1.61</v>
-      </c>
-      <c r="E4" s="1">
-        <v>13.64</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2.06</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.65</v>
-      </c>
-      <c r="E5" s="1">
-        <v>16.45</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3323,9 +3310,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3546,27 +3536,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3591,9 +3569,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
increased version number to 0.0.4 worked on better assignment between data and expected molecule fixed crash when opening excel file that is already open by excel Added some new example problems
</commit_message>
<xml_diff>
--- a/exampleProblems/ch9_016/ch9_016.xlsx
+++ b/exampleProblems/ch9_016/ch9_016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/ch9_016/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_5573853B0C84BB957DF9412134EB6A4605B0F9D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA167CDF-6601-4377-9719-43B21577D9CC}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="11_5573853B0C84BB957DF9412134EB6A4605B0F9D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58628345-DAFF-447F-AA51-A3276612A182}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="1650" windowWidth="23880" windowHeight="13620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="450" windowWidth="23295" windowHeight="13620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -623,7 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1382,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,6 +1464,7 @@
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="6"/>
+      <c r="L2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="6"/>
     </row>
@@ -1497,7 +1498,6 @@
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="6"/>
     </row>
@@ -1531,7 +1531,6 @@
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="6"/>
     </row>
@@ -1565,7 +1564,6 @@
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="6"/>
     </row>
@@ -1599,7 +1597,6 @@
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="6"/>
     </row>
@@ -1798,8 +1795,8 @@
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="6"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="6"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="9"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -1831,8 +1828,17 @@
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="6"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="9"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
@@ -1844,10 +1850,6 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="6"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="6"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
@@ -1859,10 +1861,6 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="6"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="6"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
@@ -1874,27 +1872,19 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="6"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="6"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="9"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="9"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1904,21 +1894,8 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="9"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1929,7 +1906,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1940,7 +1917,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1951,7 +1928,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1962,7 +1939,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1973,7 +1950,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1984,7 +1961,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1995,7 +1972,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2006,7 +1983,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2017,18 +1994,18 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2039,71 +2016,16 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3263,10 +3185,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0628732-26E0-6345-9202-8A755BCBA328}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection sqref="A1:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3304,21 +3226,384 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F2" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G2" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F3" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G3" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F4" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G4" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F5" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G5" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.11</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F6" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G6" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F7" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G7" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F8" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F9" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G9" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.11</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F10" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G10" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F11" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G11" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F12" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G12" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F13" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="G13" s="1">
+        <v>24.96</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100155B07917A39914F9664B9093559A33D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fbeff89c08116489e82681c46e7ae15d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f6191221-55a2-427d-afce-6bfcc029a585" xmlns:ns4="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a905948312a67a3512ded1d64743b24d" ns3:_="" ns4:_="">
     <xsd:import namespace="f6191221-55a2-427d-afce-6bfcc029a585"/>
@@ -3535,6 +3820,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3542,14 +3836,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCEF473A-5319-4ED2-888F-44217AC86176}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3564,6 +3850,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added ability to sync from MestReNova
</commit_message>
<xml_diff>
--- a/exampleProblems/ch9_016/ch9_016.xlsx
+++ b/exampleProblems/ch9_016/ch9_016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/ch9_016/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_5573853B0C84BB957DF9412134EB6A4605B0F9D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58628345-DAFF-447F-AA51-A3276612A182}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="11_5573853B0C84BB957DF9412134EB6A4605B0F9D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22EBDB54-1F30-4CE1-B286-5C97B77D9A02}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="450" windowWidth="23295" windowHeight="13620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3750" yWindow="30" windowWidth="19260" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -586,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1384,7 +1384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:K13"/>
     </sheetView>
   </sheetViews>
@@ -3188,7 +3188,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K13"/>
+      <selection activeCell="A2" sqref="A2:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3227,374 +3227,158 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>3.75</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3.75</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F2" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G2" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2.34</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2.34</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F3" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G3" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2.11</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2.11</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F4" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G4" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2.06</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2.06</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F5" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G5" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3.75</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.11</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F6" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G6" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2.11</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3.75</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F7" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G7" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3.75</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2.06</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F8" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G8" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2.06</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3.75</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F9" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G9" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2.34</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2.11</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F10" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G10" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2.11</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2.34</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F11" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G11" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2.34</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2.06</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F12" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G12" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A12" s="5"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2.06</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2.34</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>6.29</v>
-      </c>
-      <c r="F13" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="G13" s="1">
-        <v>24.96</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A13" s="5"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="6"/>
     </row>
@@ -3604,6 +3388,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100155B07917A39914F9664B9093559A33D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fbeff89c08116489e82681c46e7ae15d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f6191221-55a2-427d-afce-6bfcc029a585" xmlns:ns4="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a905948312a67a3512ded1d64743b24d" ns3:_="" ns4:_="">
     <xsd:import namespace="f6191221-55a2-427d-afce-6bfcc029a585"/>
@@ -3820,22 +3619,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCEF473A-5319-4ED2-888F-44217AC86176}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3852,29 +3661,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>